<commit_message>
filled in table for ANN & SVM
</commit_message>
<xml_diff>
--- a/Classifiers/Figures/AccuracySummaryTable.xlsx
+++ b/Classifiers/Figures/AccuracySummaryTable.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,6 +468,14 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
+      <c r="C5" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2">
+        <v>0.2893</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -476,6 +484,14 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
+      <c r="C6" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
filled in table - ALL
</commit_message>
<xml_diff>
--- a/Classifiers/Figures/AccuracySummaryTable.xlsx
+++ b/Classifiers/Figures/AccuracySummaryTable.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,11 +439,15 @@
       <c r="C3" s="2">
         <v>0.92400000000000004</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2">
+        <v>0.98040000000000005</v>
+      </c>
       <c r="E3" s="2">
         <v>0.99099999999999999</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="2">
+        <v>0.99129999999999996</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -455,11 +459,15 @@
       <c r="C4" s="2">
         <v>0.95799999999999996</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2">
+        <v>0.9677</v>
+      </c>
       <c r="E4" s="2">
         <v>0.96650000000000003</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="2">
+        <v>0.95779999999999998</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -471,11 +479,15 @@
       <c r="C5" s="2">
         <v>0.74</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2">
+        <v>0.28770000000000001</v>
+      </c>
       <c r="E5" s="2">
         <v>0.2893</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="2">
+        <v>0.14430000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -487,11 +499,15 @@
       <c r="C6" s="2">
         <v>0.75900000000000001</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2">
+        <v>0.1784</v>
+      </c>
       <c r="E6" s="2">
         <v>7.9299999999999995E-2</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="2">
+        <v>0.20780000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -503,11 +519,15 @@
       <c r="C7" s="2">
         <v>0.94899999999999995</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2">
+        <v>0.9657</v>
+      </c>
       <c r="E7" s="2">
         <v>0.98</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="2">
+        <v>0.99199999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>